<commit_message>
Agregar varios Ejemplos y Correciones en los perfiles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CodigoPaises.xlsx
+++ b/output/StructureDefinition-CodigoPaises.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-21T18:30:18-04:00</t>
+    <t>2024-06-23T21:41:08-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -135,7 +135,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Address.country</t>
+    <t>element:Element</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>